<commit_message>
commit after making changes to freelisting
</commit_message>
<xml_diff>
--- a/src/test/resources/excel.xlsx
+++ b/src/test/resources/excel.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2408719\IdeaProjects\CarWashServices\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25D82E84-FB6D-4E22-A2C4-EE53A4450042}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4F0631C-DCA3-43AF-A5C9-CCAFBDDA8307}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -345,10 +345,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:A7"/>
+  <dimension ref="A2:A8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -386,6 +386,11 @@
         <v>10</v>
       </c>
     </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>376836</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>